<commit_message>
added model2 for training
</commit_message>
<xml_diff>
--- a/exploitabilityTesting/results.xlsx
+++ b/exploitabilityTesting/results.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Iterations</t>
   </si>
@@ -23,6 +23,12 @@
   </si>
   <si>
     <t>EXP-P2</t>
+  </si>
+  <si>
+    <t>Valores son avg r from P1 perspective</t>
+  </si>
+  <si>
+    <t>MODEL1</t>
   </si>
 </sst>
 </file>
@@ -364,15 +370,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D3"/>
+  <dimension ref="B1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -382,16 +393,330 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1000000</v>
       </c>
       <c r="C3">
-        <v>-2.8</v>
+        <v>-1.79</v>
       </c>
       <c r="D3">
-        <v>3.52</v>
+        <v>3.12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2000000</v>
+      </c>
+      <c r="C4">
+        <v>-1.1499999999999999</v>
+      </c>
+      <c r="D4">
+        <v>1.28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>3000000</v>
+      </c>
+      <c r="C5">
+        <v>-0.56999999999999995</v>
+      </c>
+      <c r="D5">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4000000</v>
+      </c>
+      <c r="C6">
+        <v>-0.46</v>
+      </c>
+      <c r="D6">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>5000000</v>
+      </c>
+      <c r="C7">
+        <v>-0.44</v>
+      </c>
+      <c r="D7">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>6000000</v>
+      </c>
+      <c r="C8">
+        <v>-0.33</v>
+      </c>
+      <c r="D8">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>7000000</v>
+      </c>
+      <c r="C9">
+        <v>-0.37</v>
+      </c>
+      <c r="D9">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>8000000</v>
+      </c>
+      <c r="C10">
+        <v>-0.38</v>
+      </c>
+      <c r="D10">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>9000000</v>
+      </c>
+      <c r="C11">
+        <v>-1.38</v>
+      </c>
+      <c r="D11">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>10000000</v>
+      </c>
+      <c r="C12">
+        <v>-0.5</v>
+      </c>
+      <c r="D12">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>11000000</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>12000000</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>13000000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>14000000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>15000000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>16000000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>17000000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>18000000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>19000000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>20000000</v>
+      </c>
+      <c r="C22">
+        <v>-0.48</v>
+      </c>
+      <c r="D22">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>21000000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>22000000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>23000000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>24000000</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>25000000</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>26000000</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>27000000</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>28000000</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>29000000</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>30000000</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>31000000</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>32000000</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>33000000</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>34000000</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>35000000</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>36000000</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>37000000</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>38000000</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>39000000</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>40000000</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>41000000</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>42000000</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>43000000</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>44000000</v>
+      </c>
+      <c r="C46">
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="D46">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>45000000</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>46000000</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>47000000</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>48000000</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>49000000</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>50000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>